<commit_message>
fixed many bugs in geom.project_polarcoord_lines work on example schoollist_1
</commit_message>
<xml_diff>
--- a/examples/catalogue_30s_1/generated_output/ALA1934_RR-excerpt.pdf.xlsx
+++ b/examples/catalogue_30s_1/generated_output/ALA1934_RR-excerpt.pdf.xlsx
@@ -6360,10 +6360,10 @@
       <c r="K95" t="s">
         <v>26</v>
       </c>
-      <c r="L95" t="s">
+      <c r="L95" t="s"/>
+      <c r="M95" t="s">
         <v>27</v>
       </c>
-      <c r="M95" t="s"/>
       <c r="N95" t="s">
         <v>28</v>
       </c>
@@ -8759,10 +8759,10 @@
       <c r="K162" t="s">
         <v>66</v>
       </c>
-      <c r="L162" t="s">
+      <c r="L162" t="s"/>
+      <c r="M162" t="s">
         <v>453</v>
       </c>
-      <c r="M162" t="s"/>
       <c r="N162" t="s">
         <v>454</v>
       </c>
@@ -8808,10 +8808,10 @@
       <c r="K163" t="s">
         <v>66</v>
       </c>
-      <c r="L163" t="s">
+      <c r="L163" t="s"/>
+      <c r="M163" t="s">
         <v>459</v>
       </c>
-      <c r="M163" t="s"/>
       <c r="N163" t="s">
         <v>108</v>
       </c>

</xml_diff>